<commit_message>
add X, minus and plus in cart checks
</commit_message>
<xml_diff>
--- a/EKrut/jabulaTests.xlsx
+++ b/EKrut/jabulaTests.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20393"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ebraude-my.sharepoint.com/personal/neta_amzalag_e_braude_ac_il/Documents/Documents/GitHub/EKrut/EKrut/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ebraude-my.sharepoint.com/personal/vital_marciano_e_braude_ac_il/Documents/Documents/GitHub/EKrut/EKrut/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="14_{A35FF41F-297D-4C5A-9D53-423832ACD0B5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{448057C6-3B96-4F64-9101-3F8BF63D3374}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="14_{A35FF41F-297D-4C5A-9D53-423832ACD0B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{448057C6-3B96-4F64-9101-3F8BF63D3374}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20736" windowHeight="11160" xr2:uid="{402B0296-DA83-4036-ACE0-01BDCEF89F96}"/>
+    <workbookView minimized="1" xWindow="7185" yWindow="4275" windowWidth="13305" windowHeight="6645" xr2:uid="{402B0296-DA83-4036-ACE0-01BDCEF89F96}"/>
   </bookViews>
   <sheets>
     <sheet name="בלי כפיליות" sheetId="3" r:id="rId1"/>
@@ -391,7 +391,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FF7030A0"/>
-        <rFont val="Calibri"/>
+        <rFont val="Arial"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -406,7 +406,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FF7030A0"/>
-        <rFont val="Calibri"/>
+        <rFont val="Arial"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -421,7 +421,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FF7030A0"/>
-        <rFont val="Calibri"/>
+        <rFont val="Arial"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -431,7 +431,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="Arial"/>
         <family val="2"/>
         <charset val="177"/>
         <scheme val="minor"/>
@@ -447,7 +447,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FF7030A0"/>
-        <rFont val="Calibri"/>
+        <rFont val="Arial"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -457,7 +457,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="Arial"/>
         <family val="2"/>
         <charset val="177"/>
         <scheme val="minor"/>
@@ -473,7 +473,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FF7030A0"/>
-        <rFont val="Calibri"/>
+        <rFont val="Arial"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -488,7 +488,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FF7030A0"/>
-        <rFont val="Calibri"/>
+        <rFont val="Arial"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -503,7 +503,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FF7030A0"/>
-        <rFont val="Calibri"/>
+        <rFont val="Arial"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -518,7 +518,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FF7030A0"/>
-        <rFont val="Calibri"/>
+        <rFont val="Arial"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -533,7 +533,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FF7030A0"/>
-        <rFont val="Calibri"/>
+        <rFont val="Arial"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -548,7 +548,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FF7030A0"/>
-        <rFont val="Calibri"/>
+        <rFont val="Arial"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -558,7 +558,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="Arial"/>
         <family val="2"/>
         <charset val="177"/>
         <scheme val="minor"/>
@@ -569,7 +569,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FF7030A0"/>
-        <rFont val="Calibri"/>
+        <rFont val="Arial"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -588,7 +588,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <charset val="177"/>
       <scheme val="minor"/>
@@ -638,14 +638,14 @@
     <font>
       <sz val="11"/>
       <color rgb="FF0070C0"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -658,7 +658,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FF7030A0"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1452,7 +1452,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1462,23 +1462,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4578AC60-054D-4D63-83A7-2DCD1DC44005}">
   <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView rightToLeft="1" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.21875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="16.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="71.6640625" style="34" customWidth="1"/>
-    <col min="6" max="6" width="44.109375" style="35" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.25" style="1" customWidth="1"/>
+    <col min="2" max="2" width="16.75" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.25" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="71.625" style="34" customWidth="1"/>
+    <col min="6" max="6" width="44.125" style="35" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="69" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="8.88671875" style="1"/>
+    <col min="8" max="16384" width="8.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="15" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1499,7 +1499,7 @@
       </c>
       <c r="G1" s="34"/>
     </row>
-    <row r="2" spans="1:7" ht="94.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" ht="94.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="12">
         <v>3</v>
       </c>
@@ -1522,7 +1522,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A3" s="12">
         <v>13</v>
       </c>
@@ -1545,7 +1545,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.2">
       <c r="A4" s="12">
         <v>23</v>
       </c>
@@ -1568,7 +1568,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.2">
       <c r="A5" s="12">
         <v>24</v>
       </c>
@@ -1591,7 +1591,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" ht="15" x14ac:dyDescent="0.2">
       <c r="A6" s="12">
         <v>34</v>
       </c>
@@ -1614,7 +1614,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" ht="15" x14ac:dyDescent="0.2">
       <c r="A7" s="12">
         <v>30</v>
       </c>
@@ -1637,7 +1637,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" ht="15" x14ac:dyDescent="0.2">
       <c r="A8" s="12">
         <v>31</v>
       </c>
@@ -1660,7 +1660,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" ht="15" x14ac:dyDescent="0.2">
       <c r="A9" s="12">
         <v>32</v>
       </c>
@@ -1681,7 +1681,7 @@
       </c>
       <c r="G9" s="64"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" ht="15" x14ac:dyDescent="0.2">
       <c r="A10" s="12">
         <v>33</v>
       </c>
@@ -1702,7 +1702,7 @@
       </c>
       <c r="G10" s="64"/>
     </row>
-    <row r="11" spans="1:7" ht="84" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" ht="84" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="9">
         <v>28</v>
       </c>
@@ -1723,7 +1723,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A12" s="9">
         <v>29</v>
       </c>
@@ -1744,7 +1744,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A13" s="9">
         <v>30</v>
       </c>
@@ -1765,7 +1765,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="43.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" ht="43.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="9">
         <v>31</v>
       </c>
@@ -1786,7 +1786,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="53">
         <v>34</v>
       </c>
@@ -1807,7 +1807,7 @@
       </c>
       <c r="G15" s="58"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="G16" s="34"/>
     </row>
   </sheetData>
@@ -1828,16 +1828,16 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.25" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="45" t="s">
         <v>0</v>
       </c>
@@ -1849,7 +1849,7 @@
       <c r="E1" s="47"/>
       <c r="F1" s="48"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" s="49"/>
       <c r="B2" s="50" t="s">
         <v>102</v>
@@ -1861,7 +1861,7 @@
       <c r="E2" s="52"/>
       <c r="F2" s="50"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="44"/>
       <c r="B3" s="43" t="s">
         <v>91</v>
@@ -1873,7 +1873,7 @@
       <c r="E3" s="43"/>
       <c r="F3" s="43"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="43"/>
       <c r="B4" s="43" t="s">
         <v>94</v>
@@ -1885,7 +1885,7 @@
       <c r="E4" s="43"/>
       <c r="F4" s="43"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="43"/>
       <c r="B5" s="43" t="s">
         <v>98</v>
@@ -1897,7 +1897,7 @@
       <c r="E5" s="43"/>
       <c r="F5" s="43"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="43"/>
       <c r="B6" s="43" t="s">
         <v>93</v>
@@ -1909,7 +1909,7 @@
       <c r="E6" s="43"/>
       <c r="F6" s="43"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="43"/>
       <c r="B7" s="43" t="s">
         <v>92</v>
@@ -1921,7 +1921,7 @@
       <c r="E7" s="43"/>
       <c r="F7" s="43"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="43"/>
       <c r="B8" s="43" t="s">
         <v>103</v>
@@ -1933,7 +1933,7 @@
       <c r="E8" s="43"/>
       <c r="F8" s="43"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="43"/>
       <c r="B9" s="43" t="s">
         <v>105</v>
@@ -1945,7 +1945,7 @@
       <c r="E9" s="43"/>
       <c r="F9" s="43"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="43"/>
       <c r="B10" s="43" t="s">
         <v>106</v>
@@ -1957,7 +1957,7 @@
       <c r="E10" s="43"/>
       <c r="F10" s="43"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="43"/>
       <c r="B11" s="43" t="s">
         <v>104</v>
@@ -1969,7 +1969,7 @@
       <c r="E11" s="43"/>
       <c r="F11" s="43"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="43"/>
       <c r="B12" s="43" t="s">
         <v>95</v>
@@ -1981,7 +1981,7 @@
       <c r="E12" s="43"/>
       <c r="F12" s="43"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="43"/>
       <c r="B13" s="43" t="s">
         <v>96</v>
@@ -1993,7 +1993,7 @@
       <c r="E13" s="43"/>
       <c r="F13" s="43"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="43"/>
       <c r="B14" s="43" t="s">
         <v>97</v>
@@ -2005,7 +2005,7 @@
       <c r="E14" s="43"/>
       <c r="F14" s="43"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="43"/>
       <c r="B15" s="43" t="s">
         <v>99</v>
@@ -2017,7 +2017,7 @@
       <c r="E15" s="43"/>
       <c r="F15" s="43"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="43"/>
       <c r="B16" s="43" t="s">
         <v>100</v>
@@ -2029,7 +2029,7 @@
       <c r="E16" s="43"/>
       <c r="F16" s="43"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="43"/>
       <c r="B17" s="43" t="s">
         <v>101</v>
@@ -2054,17 +2054,17 @@
       <selection activeCell="E40" sqref="E40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.21875" customWidth="1"/>
-    <col min="2" max="2" width="16.77734375" style="42" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.77734375" customWidth="1"/>
-    <col min="4" max="4" width="16.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="130.77734375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="44.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.25" customWidth="1"/>
+    <col min="2" max="2" width="16.75" style="42" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.75" customWidth="1"/>
+    <col min="4" max="4" width="16.125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="130.75" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="44.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -2084,7 +2084,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" s="11">
         <v>1</v>
       </c>
@@ -2104,7 +2104,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" s="12">
         <v>2</v>
       </c>
@@ -2124,7 +2124,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" s="12">
         <v>3</v>
       </c>
@@ -2144,7 +2144,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A5" s="12">
         <v>4</v>
       </c>
@@ -2162,7 +2162,7 @@
       </c>
       <c r="F5" s="18"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A6" s="12">
         <v>5</v>
       </c>
@@ -2182,7 +2182,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A7" s="12">
         <v>6</v>
       </c>
@@ -2202,7 +2202,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A8" s="12">
         <v>7</v>
       </c>
@@ -2222,7 +2222,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A9" s="12">
         <v>8</v>
       </c>
@@ -2242,7 +2242,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A10" s="12">
         <v>9</v>
       </c>
@@ -2262,7 +2262,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A11" s="12">
         <v>10</v>
       </c>
@@ -2282,7 +2282,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A12" s="12">
         <v>11</v>
       </c>
@@ -2302,7 +2302,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A13" s="12">
         <v>12</v>
       </c>
@@ -2322,7 +2322,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A14" s="12">
         <v>13</v>
       </c>
@@ -2342,7 +2342,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="13">
         <v>14</v>
       </c>
@@ -2362,7 +2362,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A16" s="11">
         <v>15</v>
       </c>
@@ -2382,7 +2382,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A17" s="12">
         <v>16</v>
       </c>
@@ -2402,7 +2402,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A18" s="12">
         <v>17</v>
       </c>
@@ -2422,7 +2422,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A19" s="12">
         <v>18</v>
       </c>
@@ -2442,7 +2442,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A20" s="12">
         <v>19</v>
       </c>
@@ -2462,7 +2462,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A21" s="12">
         <v>20</v>
       </c>
@@ -2482,7 +2482,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A22" s="12">
         <v>21</v>
       </c>
@@ -2502,7 +2502,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A23" s="12">
         <v>22</v>
       </c>
@@ -2522,7 +2522,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A24" s="12">
         <v>23</v>
       </c>
@@ -2542,7 +2542,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A25" s="12">
         <v>24</v>
       </c>
@@ -2562,7 +2562,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A26" s="12">
         <v>25</v>
       </c>
@@ -2582,7 +2582,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A27" s="12">
         <v>26</v>
       </c>
@@ -2602,7 +2602,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A28" s="12">
         <v>27</v>
       </c>
@@ -2622,7 +2622,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A29" s="12">
         <v>28</v>
       </c>
@@ -2642,7 +2642,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A30" s="12">
         <v>29</v>
       </c>
@@ -2662,7 +2662,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A31" s="12">
         <v>30</v>
       </c>
@@ -2682,7 +2682,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A32" s="12">
         <v>31</v>
       </c>
@@ -2702,7 +2702,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A33" s="12">
         <v>32</v>
       </c>
@@ -2722,7 +2722,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A34" s="12">
         <v>33</v>
       </c>
@@ -2742,7 +2742,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A35" s="12">
         <v>34</v>
       </c>
@@ -2762,7 +2762,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A36" s="12">
         <v>35</v>
       </c>
@@ -2782,7 +2782,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A37" s="12">
         <v>36</v>
       </c>
@@ -2802,7 +2802,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A38" s="12">
         <v>37</v>
       </c>
@@ -2822,7 +2822,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A39" s="13">
         <v>38</v>
       </c>
@@ -2842,7 +2842,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A40" s="14">
         <v>39</v>
       </c>
@@ -2862,7 +2862,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A41" s="12">
         <v>40</v>
       </c>
@@ -2882,7 +2882,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A42" s="15">
         <v>41</v>
       </c>
@@ -2902,7 +2902,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A43" s="12">
         <v>42</v>
       </c>
@@ -2922,7 +2922,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A44" s="15">
         <v>43</v>
       </c>
@@ -2942,7 +2942,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A45" s="12">
         <v>44</v>
       </c>
@@ -2962,7 +2962,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A46" s="15">
         <v>45</v>
       </c>
@@ -2982,7 +2982,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="47" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A47" s="13">
         <v>46</v>
       </c>
@@ -3002,7 +3002,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="48" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A48" s="16">
         <v>47</v>
       </c>
@@ -3258,18 +3258,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3292,14 +3292,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{34A5AF2E-90FB-4221-AD46-D1DDBA68F77C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{59C1BE13-2117-4113-8677-6FB0C00BD944}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
@@ -3314,4 +3306,12 @@
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{34A5AF2E-90FB-4221-AD46-D1DDBA68F77C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>